<commit_message>
Minor fixes and changes for v1.1
See v1.1. changes.txt for full details.
</commit_message>
<xml_diff>
--- a/ManufactureInfoV1_0s/BOM.xlsx
+++ b/ManufactureInfoV1_0s/BOM.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schuyler\Documents\Eagle\Projects\FastDataAcquisition\ManufactureInfoV1_0s\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="720" yWindow="420" windowWidth="27555" windowHeight="12555"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="304">
   <si>
     <t>Parts</t>
   </si>
@@ -166,9 +171,6 @@
     <t>Polarized capacitors.</t>
   </si>
   <si>
-    <t>R3, R5, R8, R21, R41, R43, R44, R47</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -232,12 +234,6 @@
     <t>R46</t>
   </si>
   <si>
-    <t>16k</t>
-  </si>
-  <si>
-    <t>1276-5091-1-ND</t>
-  </si>
-  <si>
     <t>C87, C90, C104</t>
   </si>
   <si>
@@ -313,12 +309,6 @@
     <t>R42</t>
   </si>
   <si>
-    <t>26.1k</t>
-  </si>
-  <si>
-    <t>1276-4779-1-ND</t>
-  </si>
-  <si>
     <t>R60, R61</t>
   </si>
   <si>
@@ -917,6 +907,30 @@
   </si>
   <si>
     <t>XCFxxS Xilinx Program Flash.</t>
+  </si>
+  <si>
+    <t>R43, R47</t>
+  </si>
+  <si>
+    <t>R3, R5, R8, R21, R41, R44</t>
+  </si>
+  <si>
+    <t>ERJ-1GEF8870C</t>
+  </si>
+  <si>
+    <t>P887ABCT-ND</t>
+  </si>
+  <si>
+    <t>2.49k</t>
+  </si>
+  <si>
+    <t>1276-4681-1-ND</t>
+  </si>
+  <si>
+    <t>1.69k</t>
+  </si>
+  <si>
+    <t>1276-3491-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1457,6 +1471,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1504,7 +1521,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1539,7 +1556,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1748,15 +1765,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="C50" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
@@ -1794,13 +1811,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" t="s">
         <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1809,7 +1826,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
         <v>43</v>
@@ -1817,13 +1834,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" t="s">
         <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1840,13 +1857,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1858,18 +1875,18 @@
         <v>805</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -1878,24 +1895,24 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
@@ -1904,7 +1921,7 @@
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H6" t="s">
         <v>13</v>
@@ -1935,16 +1952,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
         <v>43</v>
@@ -2024,13 +2041,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -2047,13 +2064,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>57</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -2070,13 +2087,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
@@ -2093,13 +2110,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -2116,13 +2133,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -2131,24 +2148,24 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H16" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -2157,24 +2174,24 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H17" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D18" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -2183,24 +2200,24 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H18" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C19" s="1">
         <v>436500212</v>
       </c>
       <c r="D19" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -2209,73 +2226,73 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D20" t="s">
+        <v>282</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>283</v>
+      </c>
+      <c r="H20" t="s">
         <v>284</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D20" t="s">
-        <v>287</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>288</v>
-      </c>
-      <c r="H20" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>173</v>
+      </c>
+      <c r="H21" t="s">
         <v>174</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D21" t="s">
-        <v>177</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>178</v>
-      </c>
-      <c r="H21" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B22" s="1">
         <v>330</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -2284,24 +2301,24 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H22" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B23" s="1">
         <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -2310,21 +2327,21 @@
         <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
@@ -2333,21 +2350,21 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
@@ -2356,18 +2373,18 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F26">
         <v>5</v>
@@ -2381,13 +2398,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -2396,7 +2413,7 @@
         <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H27" t="s">
         <v>17</v>
@@ -2404,13 +2421,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D28" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -2419,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H28" t="s">
         <v>17</v>
@@ -2427,13 +2444,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" t="s">
         <v>69</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
@@ -2442,7 +2459,7 @@
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H29" t="s">
         <v>17</v>
@@ -2450,14 +2467,14 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="D30" t="s">
         <v>66</v>
       </c>
-      <c r="D30" t="s">
-        <v>67</v>
-      </c>
       <c r="E30" t="s">
         <v>11</v>
       </c>
@@ -2465,7 +2482,7 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H30" t="s">
         <v>17</v>
@@ -2473,13 +2490,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -2488,7 +2505,7 @@
         <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H31" t="s">
         <v>17</v>
@@ -2496,13 +2513,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
@@ -2511,7 +2528,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H32" t="s">
         <v>17</v>
@@ -2519,13 +2536,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -2534,7 +2551,7 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H33" t="s">
         <v>17</v>
@@ -2568,16 +2585,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" t="s">
         <v>52</v>
-      </c>
-      <c r="D35" t="s">
-        <v>53</v>
       </c>
       <c r="E35" t="s">
         <v>11</v>
@@ -2586,7 +2603,7 @@
         <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H35" t="s">
         <v>17</v>
@@ -2594,16 +2611,16 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -2646,13 +2663,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
@@ -2661,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H38" t="s">
         <v>17</v>
@@ -2669,13 +2686,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D39" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E39" t="s">
         <v>11</v>
@@ -2684,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H39" t="s">
         <v>17</v>
@@ -2692,13 +2709,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D40" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E40" t="s">
         <v>11</v>
@@ -2707,7 +2724,7 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H40" t="s">
         <v>17</v>
@@ -2715,16 +2732,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B41" s="1">
         <v>330</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D41" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E41" t="s">
         <v>11</v>
@@ -2733,7 +2750,7 @@
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H41" t="s">
         <v>17</v>
@@ -2741,16 +2758,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B42" s="1">
         <v>50</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D42" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E42" t="s">
         <v>11</v>
@@ -2759,7 +2776,7 @@
         <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H42" t="s">
         <v>17</v>
@@ -2767,13 +2784,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>99</v>
+        <v>300</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>301</v>
       </c>
       <c r="E43" t="s">
         <v>11</v>
@@ -2790,22 +2807,25 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>296</v>
+      </c>
+      <c r="B44" s="1">
+        <v>887</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>299</v>
       </c>
       <c r="E44" t="s">
         <v>11</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H44" t="s">
         <v>17</v>
@@ -2813,25 +2833,22 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>30</v>
+        <v>302</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>303</v>
       </c>
       <c r="E45" t="s">
         <v>11</v>
       </c>
       <c r="F45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H45" t="s">
         <v>17</v>
@@ -2839,22 +2856,25 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="1">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="E46" t="s">
         <v>11</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G46" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H46" t="s">
         <v>17</v>
@@ -2862,22 +2882,22 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="B47" s="1">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
         <v>11</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="H47" t="s">
         <v>17</v>
@@ -2885,22 +2905,22 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>113</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
+      </c>
+      <c r="B48" s="1">
+        <v>27</v>
       </c>
       <c r="D48" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="E48" t="s">
         <v>11</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H48" t="s">
         <v>17</v>
@@ -2908,25 +2928,22 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="D49" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="E49" t="s">
         <v>11</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="H49" t="s">
         <v>17</v>
@@ -2934,42 +2951,42 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>267</v>
+        <v>121</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>268</v>
+        <v>122</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>269</v>
+        <v>123</v>
       </c>
       <c r="D50" t="s">
-        <v>270</v>
+        <v>124</v>
       </c>
       <c r="E50" t="s">
         <v>11</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>269</v>
+        <v>53</v>
       </c>
       <c r="H50" t="s">
-        <v>271</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>262</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>164</v>
+        <v>263</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>165</v>
+        <v>264</v>
       </c>
       <c r="D51" t="s">
-        <v>166</v>
+        <v>265</v>
       </c>
       <c r="E51" t="s">
         <v>11</v>
@@ -2978,24 +2995,24 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>167</v>
+        <v>264</v>
       </c>
       <c r="H51" t="s">
-        <v>168</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>278</v>
+        <v>158</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>279</v>
+        <v>159</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>280</v>
+        <v>160</v>
       </c>
       <c r="D52" t="s">
-        <v>281</v>
+        <v>161</v>
       </c>
       <c r="E52" t="s">
         <v>11</v>
@@ -3004,24 +3021,24 @@
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>282</v>
+        <v>162</v>
       </c>
       <c r="H52" t="s">
-        <v>283</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>180</v>
+        <v>273</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>181</v>
+        <v>274</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>182</v>
+        <v>275</v>
       </c>
       <c r="D53" t="s">
-        <v>183</v>
+        <v>276</v>
       </c>
       <c r="E53" t="s">
         <v>11</v>
@@ -3030,24 +3047,24 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>184</v>
+        <v>277</v>
       </c>
       <c r="H53" t="s">
-        <v>185</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D54" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E54" t="s">
         <v>11</v>
@@ -3056,24 +3073,24 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="H54" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>295</v>
+        <v>164</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>296</v>
+        <v>165</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>297</v>
+        <v>165</v>
       </c>
       <c r="D55" t="s">
-        <v>298</v>
+        <v>166</v>
       </c>
       <c r="E55" t="s">
         <v>11</v>
@@ -3082,24 +3099,24 @@
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>299</v>
+        <v>167</v>
       </c>
       <c r="H55" t="s">
-        <v>300</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>290</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>195</v>
+        <v>291</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>196</v>
+        <v>292</v>
       </c>
       <c r="D56" t="s">
-        <v>197</v>
+        <v>293</v>
       </c>
       <c r="E56" t="s">
         <v>11</v>
@@ -3108,24 +3125,24 @@
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>198</v>
+        <v>294</v>
       </c>
       <c r="H56" t="s">
-        <v>199</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>290</v>
+        <v>189</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>291</v>
+        <v>190</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>291</v>
+        <v>191</v>
       </c>
       <c r="D57" t="s">
-        <v>292</v>
+        <v>192</v>
       </c>
       <c r="E57" t="s">
         <v>11</v>
@@ -3134,24 +3151,24 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>293</v>
+        <v>193</v>
       </c>
       <c r="H57" t="s">
-        <v>294</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>245</v>
+        <v>285</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>246</v>
+        <v>286</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>247</v>
+        <v>286</v>
       </c>
       <c r="D58" t="s">
-        <v>248</v>
+        <v>287</v>
       </c>
       <c r="E58" t="s">
         <v>11</v>
@@ -3160,24 +3177,24 @@
         <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>249</v>
+        <v>288</v>
       </c>
       <c r="H58" t="s">
-        <v>250</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="D59" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E59" t="s">
         <v>11</v>
@@ -3186,24 +3203,24 @@
         <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="H59" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="D60" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="E60" t="s">
         <v>11</v>
@@ -3212,24 +3229,24 @@
         <v>1</v>
       </c>
       <c r="G60" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H60" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="D61" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="E61" t="s">
         <v>11</v>
@@ -3238,24 +3255,24 @@
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H61" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>253</v>
+        <v>226</v>
       </c>
       <c r="D62" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="E62" t="s">
         <v>11</v>
@@ -3264,24 +3281,24 @@
         <v>1</v>
       </c>
       <c r="G62" t="s">
-        <v>255</v>
+        <v>228</v>
       </c>
       <c r="H62" t="s">
-        <v>256</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="D63" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="E63" t="s">
         <v>11</v>
@@ -3290,24 +3307,24 @@
         <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
       <c r="H63" t="s">
-        <v>222</v>
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D64" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E64" t="s">
         <v>11</v>
@@ -3316,73 +3333,76 @@
         <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="H64" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>272</v>
+        <v>218</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>273</v>
+        <v>219</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>274</v>
+        <v>220</v>
       </c>
       <c r="D65" t="s">
-        <v>275</v>
+        <v>221</v>
       </c>
       <c r="E65" t="s">
         <v>11</v>
       </c>
       <c r="F65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>276</v>
+        <v>222</v>
       </c>
       <c r="H65" t="s">
-        <v>277</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>200</v>
+        <v>267</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C66" s="1">
-        <v>15912080</v>
+        <v>268</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="D66" t="s">
-        <v>202</v>
+        <v>270</v>
       </c>
       <c r="E66" t="s">
         <v>11</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G66" t="s">
-        <v>203</v>
+        <v>271</v>
+      </c>
+      <c r="H66" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>160</v>
+        <v>196</v>
       </c>
       <c r="C67" s="1">
-        <v>878321420</v>
+        <v>15912080</v>
       </c>
       <c r="D67" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="E67" t="s">
         <v>11</v>
@@ -3391,88 +3411,111 @@
         <v>1</v>
       </c>
       <c r="G67" t="s">
-        <v>160</v>
-      </c>
-      <c r="H67" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>261</v>
+        <v>154</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>263</v>
+        <v>155</v>
+      </c>
+      <c r="C68" s="1">
+        <v>878321420</v>
       </c>
       <c r="D68" t="s">
-        <v>263</v>
+        <v>156</v>
       </c>
       <c r="E68" t="s">
-        <v>264</v>
+        <v>11</v>
       </c>
       <c r="F68">
         <v>1</v>
       </c>
       <c r="G68" t="s">
-        <v>265</v>
+        <v>155</v>
       </c>
       <c r="H68" t="s">
-        <v>266</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>33</v>
+        <v>256</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>34</v>
+        <v>257</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>35</v>
+        <v>258</v>
       </c>
       <c r="D69" t="s">
-        <v>36</v>
+        <v>258</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>259</v>
       </c>
       <c r="F69">
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>37</v>
+        <v>260</v>
       </c>
       <c r="H69" t="s">
-        <v>38</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>189</v>
+        <v>33</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D70" t="s">
+        <v>36</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D71" t="s">
+        <v>186</v>
+      </c>
+      <c r="E71" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71" t="s">
         <v>187</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D70" t="s">
-        <v>191</v>
-      </c>
-      <c r="E70" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70">
-        <v>1</v>
-      </c>
-      <c r="G70" t="s">
-        <v>192</v>
-      </c>
-      <c r="H70" t="s">
-        <v>193</v>
+      <c r="H71" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>